<commit_message>
Prettier printing of tables
</commit_message>
<xml_diff>
--- a/Sales.xlsx
+++ b/Sales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dnbar\Dropbox\OAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{19215551-2EBA-46D7-9752-DAF898ED6A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05083FE5-7683-AD4C-B1D4-B107B17BBA7C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3657CE98-99B2-4EA2-A361-3CF5F23F979F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10800" xr2:uid="{0108B83E-3C77-4B82-A22E-E5E672BBCD30}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="73">
   <si>
     <t>Price</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>replied but no bank details yet</t>
   </si>
 </sst>
 </file>
@@ -644,19 +647,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19E7F62F-ABDB-4DF3-BDD6-D73ED295D066}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="11.56640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.52734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -679,7 +682,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>41</v>
       </c>
@@ -699,8 +702,11 @@
       <c r="G2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>26</v>
       </c>
@@ -724,7 +730,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -748,7 +754,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -772,7 +778,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>32</v>
       </c>
@@ -796,7 +802,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -820,7 +826,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -844,7 +850,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -868,7 +874,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>35</v>
       </c>
@@ -892,7 +898,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
@@ -916,7 +922,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>56</v>
       </c>
@@ -940,7 +946,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>44</v>
       </c>
@@ -964,7 +970,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>5</v>
       </c>
@@ -988,7 +994,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
@@ -1012,7 +1018,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>62</v>
       </c>
@@ -1036,7 +1042,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
@@ -1060,7 +1066,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1084,7 +1090,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>65</v>
       </c>
@@ -1108,7 +1114,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1132,7 +1138,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>59</v>
       </c>
@@ -1156,7 +1162,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>50</v>
       </c>
@@ -1177,7 +1183,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="H23">
         <f>COUNTA(H2:H22)</f>
         <v>19</v>

</xml_diff>